<commit_message>
working with merge_cells and unmerge_cells
</commit_message>
<xml_diff>
--- a/Munaf.xlsx
+++ b/Munaf.xlsx
@@ -427,21 +427,6 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>working</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>with</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
           <t>openpyxl</t>

</xml_diff>

<commit_message>
working with insert and delete
</commit_message>
<xml_diff>
--- a/Munaf.xlsx
+++ b/Munaf.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,7 +427,7 @@
           <t>I</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -439,22 +439,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -466,22 +466,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -493,22 +493,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -520,22 +520,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -547,22 +547,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -574,22 +574,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -601,184 +601,54 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>openpyxl</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>working</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>with</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>openpyxl</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>working</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>with</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>openpyxl</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>working</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>with</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>openpyxl</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>working</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>with</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>openpyxl</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>I</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>working</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>with</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>openpyxl</t>
-        </is>
-      </c>
-    </row>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>openpyxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -790,22 +660,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -817,22 +687,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -844,22 +714,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -871,22 +741,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -898,22 +768,22 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>
@@ -925,22 +795,130 @@
           <t>I</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>am</t>
-        </is>
-      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>working</t>
+          <t>am</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>with</t>
+          <t>working</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>openpyxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>am</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>openpyxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>am</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>openpyxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>am</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>openpyxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>am</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
         <is>
           <t>openpyxl</t>
         </is>

</xml_diff>